<commit_message>
removed case sensitivity and made a more practical test card file
</commit_message>
<xml_diff>
--- a/data/TestCards.xlsx
+++ b/data/TestCards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>front</t>
   </si>
@@ -22,10 +22,28 @@
     <t>back</t>
   </si>
   <si>
-    <t>frontTest</t>
-  </si>
-  <si>
-    <t>backTest</t>
+    <t>가게</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>아마도</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>안녕</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>가금</t>
+  </si>
+  <si>
+    <t>Sometimes</t>
   </si>
 </sst>
 </file>
@@ -75,13 +93,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,14 +406,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -404,11 +425,35 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no longer displays same card twice in a row
</commit_message>
<xml_diff>
--- a/data/TestCards.xlsx
+++ b/data/TestCards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>front</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>죄송합니다</t>
+  </si>
+  <si>
+    <t>Sorry</t>
+  </si>
+  <si>
+    <t>주세요</t>
+  </si>
+  <si>
+    <t>Please</t>
+  </si>
+  <si>
+    <t>안녕하세요</t>
+  </si>
+  <si>
+    <t>Hello</t>
   </si>
   <si>
     <t>가금</t>
@@ -51,7 +69,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +81,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -93,9 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -406,14 +433,14 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -449,11 +476,35 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="21">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now allows for the front and back of the card to be swapped
</commit_message>
<xml_diff>
--- a/data/TestCards.xlsx
+++ b/data/TestCards.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>front</t>
   </si>
@@ -56,6 +56,18 @@
   </si>
   <si>
     <t>Hello</t>
+  </si>
+  <si>
+    <t>바보</t>
+  </si>
+  <si>
+    <t>Fool</t>
+  </si>
+  <si>
+    <t>고양이</t>
+  </si>
+  <si>
+    <t>Cat</t>
   </si>
   <si>
     <t>고맙습니다</t>
@@ -448,7 +460,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -490,44 +502,60 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="21">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="21">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="21">
-      <c r="A9" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="21">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>